<commit_message>
not sure what I've done, but I want to save it anyway.
</commit_message>
<xml_diff>
--- a/Logs/manual data.xlsx
+++ b/Logs/manual data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">Temp in F about 1 minute after heater shut off. Units are centers of ~8inch boards that form ceiling. </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>Heater off Thu Feb 16 00:20:18 PST 2012</t>
+  </si>
+  <si>
+    <t>Changed fan angle late night feb 18. Returned fan to previous angle around noon feb 19.</t>
+  </si>
+  <si>
+    <t>Disconnected XXXL capacitor Sun Feb 19 around 7:20</t>
+  </si>
+  <si>
+    <t>Opened window Feb 22 about 11:35AM</t>
   </si>
 </sst>
 </file>
@@ -503,11 +512,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="356266184"/>
-        <c:axId val="356269160"/>
+        <c:axId val="256250824"/>
+        <c:axId val="256278408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="356266184"/>
+        <c:axId val="256250824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -516,7 +525,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="356269160"/>
+        <c:crossAx val="256278408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -524,7 +533,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="356269160"/>
+        <c:axId val="256278408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="70.0"/>
@@ -536,14 +545,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="356266184"/>
+        <c:crossAx val="256250824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -913,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1233,6 +1241,21 @@
         <v>21</v>
       </c>
     </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>